<commit_message>
T460 - joi 16 iunie 2022, 21:04:48 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_mai_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_mai_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,16 +70,25 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Apahida</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
     <t>Cluj-Baia-Mare</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Cmp. Turzii</t>
-  </si>
-  <si>
-    <t>Cluj-Bistrita</t>
+    <t>Cluj-Satu-Mare</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
   </si>
   <si>
     <t>Acasa-Birou</t>
@@ -89,21 +98,6 @@
   </si>
   <si>
     <t>Cluj-Dej</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Zalau</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -629,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>117069</v>
+        <v>137862</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -661,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>356</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -675,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>152</v>
+        <v>47</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
@@ -689,7 +683,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="4">
-        <v>257</v>
+        <v>92</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>20</v>
@@ -713,13 +707,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -747,10 +741,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>101</v>
+        <v>421</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>18</v>
@@ -761,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>421</v>
+        <v>121</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>18</v>
@@ -775,10 +769,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="4">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>18</v>
@@ -789,13 +783,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
@@ -803,7 +797,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="4">
-        <v>47</v>
+        <v>101</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>26</v>
@@ -837,10 +831,10 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>152</v>
+        <v>421</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>18</v>
@@ -851,13 +845,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -865,13 +859,13 @@
         <v>18</v>
       </c>
       <c r="B31" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="20" customHeight="1">
@@ -882,10 +876,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="20" customHeight="1">
@@ -893,13 +887,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -930,10 +924,10 @@
         <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -944,10 +938,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -955,10 +949,10 @@
         <v>25</v>
       </c>
       <c r="B38" s="4">
-        <v>47</v>
+        <v>421</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>18</v>
@@ -969,13 +963,13 @@
         <v>26</v>
       </c>
       <c r="B39" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="20" customHeight="1">
@@ -983,10 +977,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>18</v>
@@ -1017,10 +1011,10 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>18</v>
@@ -1031,59 +1025,59 @@
         <v>31</v>
       </c>
       <c r="B44" s="4">
-        <v>30</v>
+        <v>356</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B45" s="4">
-        <v>2962</v>
+        <v>2947</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="20" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B46" s="4">
-        <v>120031</v>
+        <v>140809</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="20" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="20" customHeight="1">
       <c r="A54" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="20" customHeight="1">
       <c r="A56" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="20" customHeight="1">
       <c r="A58" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T460 -  vineri 17 iunie 2022, 08:41:01 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_mai_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_mai_2022_Alex_Bora.xlsx
@@ -70,34 +70,34 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
+    <t>Cluj-Cluj</t>
+  </si>
+  <si>
+    <t>Interes Serviciu</t>
+  </si>
+  <si>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
+  </si>
+  <si>
+    <t>Cluj-Dej</t>
+  </si>
+  <si>
+    <t>Cluj-Cmp. Turzii</t>
+  </si>
+  <si>
+    <t>Cluj-Bistrita</t>
+  </si>
+  <si>
     <t>Cluj-Apahida</t>
   </si>
   <si>
-    <t>Interes Serviciu</t>
-  </si>
-  <si>
-    <t>Cluj-Cluj</t>
-  </si>
-  <si>
-    <t>Cluj-Bontida</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Turda</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Cluj-Dej</t>
+    <t>Cluj-Zalau</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -623,7 +623,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>137862</v>
+        <v>140809</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -655,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -669,13 +669,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -683,13 +683,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>356</v>
+        <v>121</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>21</v>
@@ -741,13 +741,13 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="20" customHeight="1">
@@ -755,10 +755,10 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>18</v>
@@ -769,10 +769,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="4">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>18</v>
@@ -783,13 +783,13 @@
         <v>12</v>
       </c>
       <c r="B25" s="4">
-        <v>30</v>
+        <v>152</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="20" customHeight="1">
@@ -797,10 +797,10 @@
         <v>13</v>
       </c>
       <c r="B26" s="4">
-        <v>101</v>
+        <v>257</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>18</v>
@@ -831,13 +831,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -845,13 +845,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -862,10 +862,10 @@
         <v>30</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="20" customHeight="1">
@@ -876,10 +876,10 @@
         <v>30</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="20" customHeight="1">
@@ -887,13 +887,13 @@
         <v>20</v>
       </c>
       <c r="B33" s="4">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -921,13 +921,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="4">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -938,10 +938,10 @@
         <v>30</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="20" customHeight="1">
@@ -949,10 +949,10 @@
         <v>25</v>
       </c>
       <c r="B38" s="4">
-        <v>421</v>
+        <v>156</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>18</v>
@@ -963,13 +963,13 @@
         <v>26</v>
       </c>
       <c r="B39" s="4">
-        <v>30</v>
+        <v>257</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="20" customHeight="1">
@@ -977,10 +977,10 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>18</v>
@@ -1011,13 +1011,13 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>92</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
@@ -1025,10 +1025,10 @@
         <v>31</v>
       </c>
       <c r="B44" s="4">
-        <v>356</v>
+        <v>85</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>18</v>
@@ -1039,7 +1039,7 @@
         <v>27</v>
       </c>
       <c r="B45" s="4">
-        <v>2947</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="20" customHeight="1">
@@ -1047,7 +1047,7 @@
         <v>28</v>
       </c>
       <c r="B46" s="4">
-        <v>140809</v>
+        <v>142629</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
T460 - sâmbătă 18 iunie 2022, 13:47:04 +0300
</commit_message>
<xml_diff>
--- a/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_mai_2022_Alex_Bora.xlsx
+++ b/SCRATCH/CLEAN/foaie_parcurs_B-151-VGT_mai_2022_Alex_Bora.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>VOLVO ROMÂNIA</t>
   </si>
@@ -70,34 +70,28 @@
     <t>Observatii utilizator</t>
   </si>
   <si>
-    <t>Cluj-Apahida</t>
+    <t>Cluj-Satu-Mare</t>
   </si>
   <si>
     <t>Interes Serviciu</t>
   </si>
   <si>
-    <t>Cluj-Bistrita</t>
+    <t>Acasa-Birou</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Cluj-Dej</t>
   </si>
   <si>
-    <t>Cluj-Satu-Mare</t>
-  </si>
-  <si>
-    <t>Cluj-Baia-Mare</t>
-  </si>
-  <si>
-    <t>Acasa-Birou</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Cluj-Zalau</t>
   </si>
   <si>
-    <t>Cluj-Cmp. Turzii</t>
+    <t>Cluj-Bontida</t>
+  </si>
+  <si>
+    <t>Cluj-Turda</t>
   </si>
   <si>
     <t>Km parcursi:</t>
@@ -623,7 +617,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>215655</v>
+        <v>229926</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20" customHeight="1">
@@ -655,7 +649,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="4">
-        <v>85</v>
+        <v>421</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>17</v>
@@ -669,13 +663,13 @@
         <v>3</v>
       </c>
       <c r="B16" s="4">
-        <v>257</v>
+        <v>30</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="20" customHeight="1">
@@ -683,13 +677,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="4">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="20" customHeight="1">
@@ -707,13 +701,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="20" customHeight="1">
@@ -741,10 +735,10 @@
         <v>9</v>
       </c>
       <c r="B22" s="4">
-        <v>356</v>
+        <v>421</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>18</v>
@@ -755,13 +749,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="4">
-        <v>30</v>
+        <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20" customHeight="1">
@@ -769,13 +763,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="4">
-        <v>30</v>
+        <v>156</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="20" customHeight="1">
@@ -783,10 +777,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="4">
-        <v>421</v>
+        <v>92</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>18</v>
@@ -800,10 +794,10 @@
         <v>30</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="20" customHeight="1">
@@ -831,13 +825,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="4">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20" customHeight="1">
@@ -845,13 +839,13 @@
         <v>17</v>
       </c>
       <c r="B30" s="4">
-        <v>30</v>
+        <v>421</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="20" customHeight="1">
@@ -859,10 +853,10 @@
         <v>18</v>
       </c>
       <c r="B31" s="4">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>18</v>
@@ -873,10 +867,10 @@
         <v>19</v>
       </c>
       <c r="B32" s="4">
-        <v>152</v>
+        <v>421</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>18</v>
@@ -890,10 +884,10 @@
         <v>30</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20" customHeight="1">
@@ -924,10 +918,10 @@
         <v>30</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20" customHeight="1">
@@ -935,10 +929,10 @@
         <v>24</v>
       </c>
       <c r="B37" s="4">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>18</v>
@@ -952,10 +946,10 @@
         <v>30</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="20" customHeight="1">
@@ -963,13 +957,13 @@
         <v>26</v>
       </c>
       <c r="B39" s="4">
-        <v>30</v>
+        <v>121</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="20" customHeight="1">
@@ -977,13 +971,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="4">
-        <v>152</v>
+        <v>30</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="20" customHeight="1">
@@ -1011,13 +1005,13 @@
         <v>30</v>
       </c>
       <c r="B43" s="4">
-        <v>421</v>
+        <v>30</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="20" customHeight="1">
@@ -1025,10 +1019,10 @@
         <v>31</v>
       </c>
       <c r="B44" s="4">
-        <v>257</v>
+        <v>92</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>18</v>
@@ -1036,48 +1030,48 @@
     </row>
     <row r="45" spans="1:4" ht="20" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B45" s="4">
-        <v>3272</v>
+        <v>2759</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="20" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B46" s="4">
-        <v>218927</v>
+        <v>232685</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="20" customHeight="1">
       <c r="A51" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="20" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="20" customHeight="1">
       <c r="A54" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="20" customHeight="1">
       <c r="A56" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="20" customHeight="1">
       <c r="A58" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>